<commit_message>
wrap up ff projects
</commit_message>
<xml_diff>
--- a/assets/raw-data/ff-projects/ff-projects.xlsx
+++ b/assets/raw-data/ff-projects/ff-projects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alik\Documents\workspace\mex-extractors\assets\raw-data\ff-projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HesseE\mex-extractors\assets\raw-data\ff-projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F698CBE-EF60-44D7-9B1E-60A8A585CA79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61669A6F-9AA6-49F0-BA0A-867A4446BDED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="15360" windowHeight="4080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
   <si>
     <t>Zuwendungs-/ Auftraggeber</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>Dr Frieda Ficticious</t>
-  </si>
-  <si>
-    <t>FG33</t>
   </si>
   <si>
     <t>Five</t>
@@ -528,7 +525,7 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2053,10 +2050,10 @@
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2:H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="14" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" style="7" customWidth="1"/>
@@ -2105,7 +2102,7 @@
     </row>
     <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="26">
         <v>1364</v>
@@ -2121,9 +2118,11 @@
         <v>13</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H2" s="31"/>
+        <v>60</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I2" s="32"/>
       <c r="J2" s="33"/>
     </row>
@@ -2145,9 +2144,11 @@
         <v>15</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="31"/>
+        <v>61</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I3" s="32"/>
       <c r="J3" s="33"/>
     </row>
@@ -2173,7 +2174,9 @@
       <c r="G4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="31"/>
+      <c r="H4" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I4" s="32"/>
       <c r="J4" s="33"/>
     </row>
@@ -2197,7 +2200,9 @@
       <c r="G5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="31"/>
+      <c r="H5" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I5" s="32"/>
       <c r="J5" s="33"/>
     </row>
@@ -2216,12 +2221,14 @@
       </c>
       <c r="E6" s="35"/>
       <c r="F6" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="31"/>
+      <c r="H6" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I6" s="32"/>
       <c r="J6" s="36"/>
     </row>
@@ -2243,9 +2250,11 @@
         <v>23</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="31"/>
+        <v>61</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I7" s="36" t="s">
         <v>24</v>
       </c>
@@ -2255,7 +2264,7 @@
     </row>
     <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="34">
         <v>1364</v>
@@ -2273,7 +2282,9 @@
       <c r="G8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="31"/>
+      <c r="H8" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I8" s="6">
         <v>43101</v>
       </c>
@@ -2296,12 +2307,14 @@
       </c>
       <c r="E9" s="35"/>
       <c r="F9" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="31"/>
+      <c r="H9" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I9" s="36"/>
       <c r="J9" s="37"/>
     </row>
@@ -2323,9 +2336,11 @@
         <v>28</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="31"/>
+        <v>40</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I10" s="36"/>
       <c r="J10" s="37"/>
     </row>
@@ -2352,7 +2367,7 @@
         <v>32</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="I11" s="6">
         <v>43101</v>
@@ -2370,16 +2385,18 @@
         <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="35"/>
       <c r="F12" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="31"/>
+      <c r="H12" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I12" s="36"/>
       <c r="J12" s="39"/>
     </row>
@@ -2394,16 +2411,18 @@
         <v>20</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="35"/>
       <c r="F13" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="31"/>
+      <c r="H13" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I13" s="36"/>
       <c r="J13" s="39"/>
     </row>
@@ -2418,16 +2437,18 @@
         <v>20</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" s="35"/>
       <c r="F14" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="31"/>
+      <c r="H14" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I14" s="36"/>
       <c r="J14" s="39"/>
     </row>
@@ -2442,16 +2463,18 @@
         <v>21</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="35"/>
       <c r="F15" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="31"/>
+      <c r="H15" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I15" s="36"/>
       <c r="J15" s="39"/>
     </row>
@@ -2460,22 +2483,24 @@
         <v>11</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3">
         <v>22</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="31"/>
+      <c r="H16" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I16" s="36"/>
       <c r="J16" s="39"/>
     </row>
@@ -2487,19 +2512,21 @@
         <v>1366</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="E17" s="35"/>
       <c r="F17" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="31"/>
+      <c r="H17" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I17" s="40"/>
       <c r="J17" s="37"/>
     </row>
@@ -2514,17 +2541,17 @@
         <v>24</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="35"/>
       <c r="F18" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="31" t="s">
         <v>49</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="31" t="s">
-        <v>50</v>
       </c>
       <c r="I18" s="40"/>
       <c r="J18" s="37"/>
@@ -2540,16 +2567,18 @@
         <v>25</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" s="35"/>
       <c r="F19" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="31"/>
+      <c r="H19" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I19" s="40"/>
       <c r="J19" s="37"/>
     </row>
@@ -2562,16 +2591,18 @@
         <v>26</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E20" s="35"/>
       <c r="F20" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="31"/>
+      <c r="H20" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I20" s="36"/>
       <c r="J20" s="39"/>
     </row>
@@ -2588,12 +2619,14 @@
       </c>
       <c r="E21" s="35"/>
       <c r="F21" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="31"/>
+      <c r="H21" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I21" s="6">
         <v>25204</v>
       </c>
@@ -2608,16 +2641,18 @@
         <v>28</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" s="35"/>
       <c r="F22" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="31"/>
+      <c r="H22" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I22" s="36"/>
       <c r="J22" s="6">
         <v>25508</v>
@@ -6864,7 +6899,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6878,7 +6913,7 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feature/mx-1671 wrap up ff projects (#260)
# PR Context
- correctly skip organizations to be excluded
- fix filter rules
- based on mex-assets branch `feature/mx-1671-wrap-up-ff-projects`
</commit_message>
<xml_diff>
--- a/assets/raw-data/ff-projects/ff-projects.xlsx
+++ b/assets/raw-data/ff-projects/ff-projects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alik\Documents\workspace\mex-extractors\assets\raw-data\ff-projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HesseE\mex-extractors\assets\raw-data\ff-projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F698CBE-EF60-44D7-9B1E-60A8A585CA79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61669A6F-9AA6-49F0-BA0A-867A4446BDED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="15360" windowHeight="4080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
   <si>
     <t>Zuwendungs-/ Auftraggeber</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>Dr Frieda Ficticious</t>
-  </si>
-  <si>
-    <t>FG33</t>
   </si>
   <si>
     <t>Five</t>
@@ -528,7 +525,7 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2053,10 +2050,10 @@
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2:H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="14" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" style="7" customWidth="1"/>
@@ -2105,7 +2102,7 @@
     </row>
     <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="26">
         <v>1364</v>
@@ -2121,9 +2118,11 @@
         <v>13</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H2" s="31"/>
+        <v>60</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I2" s="32"/>
       <c r="J2" s="33"/>
     </row>
@@ -2145,9 +2144,11 @@
         <v>15</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="31"/>
+        <v>61</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I3" s="32"/>
       <c r="J3" s="33"/>
     </row>
@@ -2173,7 +2174,9 @@
       <c r="G4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="31"/>
+      <c r="H4" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I4" s="32"/>
       <c r="J4" s="33"/>
     </row>
@@ -2197,7 +2200,9 @@
       <c r="G5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="31"/>
+      <c r="H5" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I5" s="32"/>
       <c r="J5" s="33"/>
     </row>
@@ -2216,12 +2221,14 @@
       </c>
       <c r="E6" s="35"/>
       <c r="F6" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="31"/>
+      <c r="H6" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I6" s="32"/>
       <c r="J6" s="36"/>
     </row>
@@ -2243,9 +2250,11 @@
         <v>23</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="31"/>
+        <v>61</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I7" s="36" t="s">
         <v>24</v>
       </c>
@@ -2255,7 +2264,7 @@
     </row>
     <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="34">
         <v>1364</v>
@@ -2273,7 +2282,9 @@
       <c r="G8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="31"/>
+      <c r="H8" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I8" s="6">
         <v>43101</v>
       </c>
@@ -2296,12 +2307,14 @@
       </c>
       <c r="E9" s="35"/>
       <c r="F9" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="31"/>
+      <c r="H9" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I9" s="36"/>
       <c r="J9" s="37"/>
     </row>
@@ -2323,9 +2336,11 @@
         <v>28</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="31"/>
+        <v>40</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I10" s="36"/>
       <c r="J10" s="37"/>
     </row>
@@ -2352,7 +2367,7 @@
         <v>32</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="I11" s="6">
         <v>43101</v>
@@ -2370,16 +2385,18 @@
         <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="35"/>
       <c r="F12" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="31"/>
+      <c r="H12" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I12" s="36"/>
       <c r="J12" s="39"/>
     </row>
@@ -2394,16 +2411,18 @@
         <v>20</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="35"/>
       <c r="F13" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="31"/>
+      <c r="H13" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I13" s="36"/>
       <c r="J13" s="39"/>
     </row>
@@ -2418,16 +2437,18 @@
         <v>20</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" s="35"/>
       <c r="F14" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="31"/>
+      <c r="H14" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I14" s="36"/>
       <c r="J14" s="39"/>
     </row>
@@ -2442,16 +2463,18 @@
         <v>21</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="35"/>
       <c r="F15" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="31"/>
+      <c r="H15" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I15" s="36"/>
       <c r="J15" s="39"/>
     </row>
@@ -2460,22 +2483,24 @@
         <v>11</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3">
         <v>22</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="31"/>
+      <c r="H16" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I16" s="36"/>
       <c r="J16" s="39"/>
     </row>
@@ -2487,19 +2512,21 @@
         <v>1366</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="E17" s="35"/>
       <c r="F17" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="31"/>
+      <c r="H17" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I17" s="40"/>
       <c r="J17" s="37"/>
     </row>
@@ -2514,17 +2541,17 @@
         <v>24</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="35"/>
       <c r="F18" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="31" t="s">
         <v>49</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="31" t="s">
-        <v>50</v>
       </c>
       <c r="I18" s="40"/>
       <c r="J18" s="37"/>
@@ -2540,16 +2567,18 @@
         <v>25</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" s="35"/>
       <c r="F19" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="31"/>
+      <c r="H19" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I19" s="40"/>
       <c r="J19" s="37"/>
     </row>
@@ -2562,16 +2591,18 @@
         <v>26</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E20" s="35"/>
       <c r="F20" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="31"/>
+      <c r="H20" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I20" s="36"/>
       <c r="J20" s="39"/>
     </row>
@@ -2588,12 +2619,14 @@
       </c>
       <c r="E21" s="35"/>
       <c r="F21" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="31"/>
+      <c r="H21" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I21" s="6">
         <v>25204</v>
       </c>
@@ -2608,16 +2641,18 @@
         <v>28</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" s="35"/>
       <c r="F22" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="31"/>
+      <c r="H22" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="I22" s="36"/>
       <c r="J22" s="6">
         <v>25508</v>
@@ -6864,7 +6899,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6878,7 +6913,7 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>